<commit_message>
KIBON-120: Kinder statistic translated - locale no longer used from LocalThreadLocal. Only in synchronous mode we access directly this language
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kinder.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kinder.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DAA5E7-F296-4A8C-ABC3-11AC5E59D00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BDE19C-0909-495C-A3B5-6B9C0CFC85DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="720" windowWidth="16380" windowHeight="8190" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -30,100 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Angebot</t>
-  </si>
-  <si>
-    <t>Periode</t>
-  </si>
-  <si>
-    <t>Von</t>
-  </si>
-  <si>
-    <t>Bis</t>
-  </si>
-  <si>
-    <t>Eingangsdatum</t>
-  </si>
-  <si>
-    <t>Verfügungsdatum</t>
-  </si>
-  <si>
-    <t>BG-ID</t>
-  </si>
-  <si>
-    <t>Kind</t>
-  </si>
-  <si>
-    <t>Gesuchsteller 1</t>
-  </si>
-  <si>
-    <t>Gesuchsteller 2</t>
-  </si>
-  <si>
-    <t>Anteil Monat</t>
-  </si>
-  <si>
-    <t>Pensum</t>
-  </si>
-  <si>
-    <t>Kosten</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Geburtsdatum</t>
-  </si>
-  <si>
-    <t>Baby-Faktor</t>
-  </si>
-  <si>
-    <t>Bis 12 Monate</t>
-  </si>
-  <si>
-    <t>13-47 Monate</t>
-  </si>
-  <si>
-    <t>48-72 Monate</t>
-  </si>
-  <si>
-    <t>Ab 73 Monate</t>
-  </si>
-  <si>
-    <t>Betreuung</t>
-  </si>
-  <si>
-    <t>Anspruchberechtigt</t>
-  </si>
-  <si>
-    <t>BG-Pensum</t>
-  </si>
-  <si>
-    <t>BG-Pensum in Stunden</t>
-  </si>
-  <si>
-    <t>BG-Monatspensum</t>
-  </si>
-  <si>
-    <t>Vollkosten</t>
-  </si>
-  <si>
-    <t>Elternbeitrag</t>
-  </si>
-  <si>
-    <t>Gutschein</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -182,9 +90,6 @@
     <t>{kindFachstelle}</t>
   </si>
   <si>
-    <t>Fachstelle</t>
-  </si>
-  <si>
     <t>{kindErwBeduerfnisse}</t>
   </si>
   <si>
@@ -221,25 +126,127 @@
     <t>{eingeschult}</t>
   </si>
   <si>
-    <t>Kinder</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>{betreuungsStatus}</t>
   </si>
   <si>
-    <t>Schulstufe</t>
-  </si>
-  <si>
-    <t>Besondere Bedürfnisse</t>
-  </si>
-  <si>
-    <t>Spricht Amtssprache</t>
-  </si>
-  <si>
     <t>{kindSprichtAmtssprache}</t>
+  </si>
+  <si>
+    <t>{institutionTitle}</t>
+  </si>
+  <si>
+    <t>{angebotTitle}</t>
+  </si>
+  <si>
+    <t>{periodeTitle}</t>
+  </si>
+  <si>
+    <t>{eingangsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{verfuegungsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{fallIdTitle}</t>
+  </si>
+  <si>
+    <t>{kinderTitle}</t>
+  </si>
+  <si>
+    <t>{parameterTitle}</t>
+  </si>
+  <si>
+    <t>{vonTitle}</t>
+  </si>
+  <si>
+    <t>{bisTitle}</t>
+  </si>
+  <si>
+    <t>{kindTitle}</t>
+  </si>
+  <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{geburtsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{fachstelleTitle}</t>
+  </si>
+  <si>
+    <t>{babyFaktorTitle}</t>
+  </si>
+  <si>
+    <t>{besonderebeduerfnisseTitle}</t>
+  </si>
+  <si>
+    <t>{sprichtAmtsspracheTitle}</t>
+  </si>
+  <si>
+    <t>{schulstufeTitle}</t>
+  </si>
+  <si>
+    <t>{bis1MonateTitle}</t>
+  </si>
+  <si>
+    <t>{bis2MonateTitle}</t>
+  </si>
+  <si>
+    <t>{bis3MonateTitle}</t>
+  </si>
+  <si>
+    <t>{abMonateTitle}</t>
+  </si>
+  <si>
+    <t>{gesuchsteller1Title}</t>
+  </si>
+  <si>
+    <t>{gesuchsteller2Title}</t>
+  </si>
+  <si>
+    <t>{betreuungVonTitle}</t>
+  </si>
+  <si>
+    <t>{betreuungBisTitle}</t>
+  </si>
+  <si>
+    <t>{anteilMonatTitle}</t>
+  </si>
+  <si>
+    <t>{betreuungTitle}</t>
+  </si>
+  <si>
+    <t>{pensumTitle}</t>
+  </si>
+  <si>
+    <t>{kostenTitle}</t>
+  </si>
+  <si>
+    <t>{anspruchberechtigtTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumStdTitle}</t>
+  </si>
+  <si>
+    <t>{bgMonatspensumTitle}</t>
+  </si>
+  <si>
+    <t>{vollkostenTitle}</t>
+  </si>
+  <si>
+    <t>{elternbeitragTitle}</t>
+  </si>
+  <si>
+    <t>{gutscheinTitle}</t>
+  </si>
+  <si>
+    <t>{statusTitle}</t>
   </si>
 </sst>
 </file>
@@ -393,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -447,35 +454,32 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -889,8 +893,8 @@
   </sheetPr>
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:37" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -934,7 +938,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -947,59 +951,59 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C4"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C5"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
     <row r="8" spans="1:37" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
+      <c r="A8" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="20"/>
@@ -1007,214 +1011,214 @@
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
-      <c r="S8" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="T8" s="34"/>
-      <c r="U8" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="V8" s="34"/>
-      <c r="W8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="29"/>
-      <c r="AA8" s="29"/>
-      <c r="AB8" s="29"/>
-      <c r="AC8" s="29"/>
-      <c r="AD8" s="29"/>
-      <c r="AE8" s="29"/>
-      <c r="AF8" s="29"/>
-      <c r="AG8" s="29"/>
-      <c r="AH8" s="29"/>
-      <c r="AI8" s="29"/>
-      <c r="AJ8" s="29"/>
+      <c r="S8" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" s="30"/>
+      <c r="U8" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="V8" s="30"/>
+      <c r="W8" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="X8" s="34"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="34"/>
+      <c r="AA8" s="34"/>
+      <c r="AB8" s="34"/>
+      <c r="AC8" s="34"/>
+      <c r="AD8" s="34"/>
+      <c r="AE8" s="34"/>
+      <c r="AF8" s="34"/>
+      <c r="AG8" s="34"/>
+      <c r="AH8" s="34"/>
+      <c r="AI8" s="34"/>
+      <c r="AJ8" s="34"/>
     </row>
     <row r="9" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="36" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="M9" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="O9" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="S9" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="T9" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="U9" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="V9" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="W9" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="X9" s="29" t="s">
-        <v>5</v>
+      <c r="N9" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S9" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="U9" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="V9" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="W9" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="X9" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="Y9" s="18"/>
       <c r="Z9" s="18"/>
-      <c r="AA9" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB9" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC9" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD9" s="29"/>
-      <c r="AE9" s="29"/>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
-      <c r="AH9" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI9" s="29"/>
-      <c r="AJ9" s="29"/>
+      <c r="AA9" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB9" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC9" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="34"/>
+      <c r="AF9" s="34"/>
+      <c r="AG9" s="34"/>
+      <c r="AH9" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="34"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
       <c r="N10" s="31"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="34"/>
       <c r="Y10" s="18" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="AA10" s="37"/>
+      <c r="AB10" s="34"/>
       <c r="AC10" s="11" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="AD10" s="11" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="AE10" s="11" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="AF10" s="11" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="AH10" s="11" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AI10" s="11" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="AJ10" s="11" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="K11" s="24" t="e">
         <f>IF(W11&lt;=EOMONTH(I11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="O11" s="24" t="e">
         <f>IF(W11&lt;=EOMONTH(I11,12),"X","")</f>
@@ -1233,22 +1237,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="U11" s="14" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="V11" s="14" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="X11" s="16" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="Y11" s="22" t="e">
         <f>NETWORKDAYS((W11-DAY(W11)+1),(EOMONTH(W11,0)))</f>
@@ -1259,52 +1263,50 @@
         <v>#VALUE!</v>
       </c>
       <c r="AA11" s="22" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="AB11" s="26" t="e">
         <f>Z11/Y11</f>
         <v>#VALUE!</v>
       </c>
       <c r="AC11" s="23" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="AD11" s="23" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="AE11" s="23" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="AF11" s="17" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="AG11" s="26" t="e">
         <f>AE11*AB11</f>
         <v>#VALUE!</v>
       </c>
       <c r="AH11" s="17" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="AI11" s="17" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="AJ11" s="27" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="AK11" s="28" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AA9:AA10"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="U9:U10"/>
     <mergeCell ref="G8:K8"/>
@@ -1321,13 +1323,15 @@
     <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="AH9:AJ9"/>
     <mergeCell ref="V9:V10"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-120: Gesuchsteller-Kinder-Betreuung statistic translated
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kinder.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kinder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BDE19C-0909-495C-A3B5-6B9C0CFC85DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0815DC1-F235-4DAC-B2E5-B14F1163CB36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="720" windowWidth="16380" windowHeight="8190" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -395,12 +395,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -420,9 +433,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -438,9 +448,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -479,6 +486,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -893,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9:AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,9 +955,9 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -978,323 +988,323 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="8" spans="1:37" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:37" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="29" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="T8" s="30"/>
-      <c r="U8" s="29" t="s">
+      <c r="T8" s="28"/>
+      <c r="U8" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="V8" s="30"/>
-      <c r="W8" s="34" t="s">
+      <c r="V8" s="28"/>
+      <c r="W8" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="34"/>
-      <c r="Z8" s="34"/>
-      <c r="AA8" s="34"/>
-      <c r="AB8" s="34"/>
-      <c r="AC8" s="34"/>
-      <c r="AD8" s="34"/>
-      <c r="AE8" s="34"/>
-      <c r="AF8" s="34"/>
-      <c r="AG8" s="34"/>
-      <c r="AH8" s="34"/>
-      <c r="AI8" s="34"/>
-      <c r="AJ8" s="34"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
+      <c r="AI8" s="32"/>
+      <c r="AJ8" s="32"/>
     </row>
     <row r="9" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="34" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="K9" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="L9" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="M9" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="O9" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="P9" s="34" t="s">
+      <c r="P9" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="Q9" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="R9" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="S9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="T9" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="U9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="V9" s="34" t="s">
+      <c r="V9" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="W9" s="34" t="s">
+      <c r="W9" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="X9" s="34" t="s">
+      <c r="X9" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="36" t="s">
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="AB9" s="34" t="s">
+      <c r="AB9" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="AC9" s="34" t="s">
+      <c r="AC9" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="AD9" s="34"/>
-      <c r="AE9" s="34"/>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="34" t="s">
+      <c r="AD9" s="32"/>
+      <c r="AE9" s="32"/>
+      <c r="AF9" s="32"/>
+      <c r="AG9" s="32"/>
+      <c r="AH9" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="AI9" s="34"/>
-      <c r="AJ9" s="34"/>
+      <c r="AI9" s="32"/>
+      <c r="AJ9" s="32"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="18" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="Z10" s="19" t="s">
+      <c r="Z10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="34"/>
-      <c r="AC10" s="11" t="s">
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AD10" s="11" t="s">
+      <c r="AD10" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AE10" s="11" t="s">
+      <c r="AE10" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="AF10" s="11" t="s">
+      <c r="AF10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="AG10" s="11" t="s">
+      <c r="AG10" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AH10" s="11" t="s">
+      <c r="AH10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AI10" s="11" t="s">
+      <c r="AI10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AJ10" s="11" t="s">
+      <c r="AJ10" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="24" t="e">
+      <c r="K11" s="22" t="e">
         <f>IF(W11&lt;=EOMONTH(I11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O11" s="24" t="e">
+      <c r="O11" s="22" t="e">
         <f>IF(W11&lt;=EOMONTH(I11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P11" s="24" t="e">
+      <c r="P11" s="22" t="e">
         <f>IF(AND(W11&gt;=EOMONTH(I11,13),W11&lt;=EOMONTH(I11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q11" s="24" t="e">
+      <c r="Q11" s="22" t="e">
         <f>IF(AND(W11&gt;=EOMONTH(I11,48),W11&lt;=EOMONTH(I11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="24" t="e">
+      <c r="R11" s="22" t="e">
         <f>IF(W11&gt;=EOMONTH(I11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="S11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="T11" s="14" t="s">
+      <c r="T11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="U11" s="14" t="s">
+      <c r="U11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="V11" s="14" t="s">
+      <c r="V11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="W11" s="16" t="s">
+      <c r="W11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="X11" s="16" t="s">
+      <c r="X11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="Y11" s="22" t="e">
+      <c r="Y11" s="20" t="e">
         <f>NETWORKDAYS((W11-DAY(W11)+1),(EOMONTH(W11,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Z11" s="22" t="e">
+      <c r="Z11" s="20" t="e">
         <f>NETWORKDAYS(W11,X11)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AA11" s="22" t="s">
+      <c r="AA11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AB11" s="26" t="e">
+      <c r="AB11" s="24" t="e">
         <f>Z11/Y11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC11" s="23" t="s">
+      <c r="AC11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="AD11" s="23" t="s">
+      <c r="AD11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AE11" s="23" t="s">
+      <c r="AE11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AF11" s="17" t="s">
+      <c r="AF11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="AG11" s="26" t="e">
+      <c r="AG11" s="24" t="e">
         <f>AE11*AB11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AH11" s="17" t="s">
+      <c r="AH11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="AI11" s="17" t="s">
+      <c r="AI11" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="AJ11" s="27" t="s">
+      <c r="AJ11" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AK11" s="28" t="s">
+      <c r="AK11" s="26" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1309,7 +1319,6 @@
     <mergeCell ref="AA9:AA10"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="U9:U10"/>
-    <mergeCell ref="G8:K8"/>
     <mergeCell ref="W8:AJ8"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
@@ -1332,6 +1341,7 @@
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E10"/>
     <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:R8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
direct-to-dev: KIBON-2760 - Kosten Titel auf Kinderstatistik anpassen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kinder.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kinder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50F6782-0E63-4223-9617-CFF82D87D891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856C464E-2948-4EE6-9DCE-D5DD0CA0C4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>{bgMonatspensumTitle}</t>
-  </si>
-  <si>
-    <t>{vollkostenTitle}</t>
   </si>
   <si>
     <t>{elternbeitragTitle}</t>
@@ -469,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -484,13 +481,13 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,51 +500,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -961,44 +945,46 @@
   </sheetPr>
   <dimension ref="A1:AT11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375"/>
-    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="1" max="2" width="20.6640625"/>
+    <col min="3" max="3" width="15.6640625" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="8" max="10" width="12.7109375"/>
-    <col min="11" max="11" width="16.7109375"/>
-    <col min="12" max="12" width="22.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="8" max="10" width="12.6640625"/>
+    <col min="11" max="11" width="16.6640625"/>
+    <col min="12" max="12" width="22.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
     <col min="15" max="15" width="22"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" customWidth="1"/>
     <col min="17" max="20" width="22"/>
-    <col min="25" max="26" width="12.7109375"/>
-    <col min="27" max="27" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625"/>
+    <col min="27" max="27" width="11.33203125" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="16" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="16" customWidth="1"/>
-    <col min="30" max="31" width="12.7109375"/>
-    <col min="32" max="32" width="12.7109375" customWidth="1"/>
-    <col min="33" max="33" width="12.28515625" customWidth="1"/>
-    <col min="34" max="34" width="16.85546875"/>
-    <col min="35" max="35" width="13.28515625" customWidth="1"/>
-    <col min="36" max="36" width="13.42578125" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375"/>
-    <col min="38" max="38" width="19.42578125"/>
-    <col min="40" max="40" width="16.85546875"/>
-    <col min="41" max="42" width="12.7109375"/>
-    <col min="43" max="43" width="12.28515625" customWidth="1"/>
-    <col min="44" max="44" width="12.7109375" customWidth="1"/>
-    <col min="45" max="45" width="12.7109375"/>
-    <col min="46" max="46" width="13.5703125" customWidth="1"/>
-    <col min="47" max="1000" width="10.5703125"/>
+    <col min="30" max="31" width="12.6640625"/>
+    <col min="32" max="32" width="12.6640625" customWidth="1"/>
+    <col min="33" max="33" width="12.33203125" customWidth="1"/>
+    <col min="34" max="34" width="16.88671875"/>
+    <col min="35" max="35" width="13.33203125" customWidth="1"/>
+    <col min="36" max="36" width="13.44140625" customWidth="1"/>
+    <col min="37" max="37" width="12.6640625"/>
+    <col min="38" max="38" width="19.44140625"/>
+    <col min="40" max="40" width="16.88671875"/>
+    <col min="41" max="42" width="12.6640625"/>
+    <col min="43" max="43" width="12.33203125" customWidth="1"/>
+    <col min="44" max="44" width="12.6640625" customWidth="1"/>
+    <col min="45" max="45" width="12.6640625"/>
+    <col min="46" max="46" width="13.5546875" customWidth="1"/>
+    <col min="47" max="1000" width="10.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -1009,10 +995,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>37</v>
       </c>
@@ -1022,11 +1008,11 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1035,7 +1021,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1030,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1056,14 +1042,14 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="8" spans="1:46" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="31" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="29" t="s">
@@ -1073,233 +1059,233 @@
         <v>34</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="30" t="s">
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="V8" s="31"/>
-      <c r="W8" s="30" t="s">
+      <c r="V8" s="28"/>
+      <c r="W8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="34" t="s">
+      <c r="X8" s="28"/>
+      <c r="Y8" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="Z8" s="34"/>
-      <c r="AA8" s="34"/>
-      <c r="AB8" s="34"/>
-      <c r="AC8" s="34"/>
-      <c r="AD8" s="34"/>
-      <c r="AE8" s="34"/>
-      <c r="AF8" s="34"/>
-      <c r="AG8" s="34"/>
-      <c r="AH8" s="34"/>
-      <c r="AI8" s="34"/>
-      <c r="AJ8" s="34"/>
-      <c r="AK8" s="34"/>
-      <c r="AL8" s="34"/>
-      <c r="AM8" s="34"/>
-      <c r="AN8" s="34"/>
-      <c r="AO8" s="34"/>
-      <c r="AP8" s="34"/>
-      <c r="AQ8" s="34"/>
-      <c r="AR8" s="34"/>
-      <c r="AS8" s="34"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="24"/>
+      <c r="AJ8" s="24"/>
+      <c r="AK8" s="24"/>
+      <c r="AL8" s="24"/>
+      <c r="AM8" s="24"/>
+      <c r="AN8" s="24"/>
+      <c r="AO8" s="24"/>
+      <c r="AP8" s="24"/>
+      <c r="AQ8" s="24"/>
+      <c r="AR8" s="24"/>
+      <c r="AS8" s="24"/>
     </row>
-    <row r="9" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
-      <c r="C9" s="33"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="M9" s="34" t="s">
+      <c r="L9" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="N9" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="O9" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="Q9" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="R9" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="S9" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="T9" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="U9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="V9" s="34" t="s">
+      <c r="V9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="W9" s="34" t="s">
+      <c r="W9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="X9" s="34" t="s">
+      <c r="X9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Y9" s="34" t="s">
+      <c r="Y9" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="Z9" s="34" t="s">
+      <c r="Z9" s="24" t="s">
         <v>56</v>
       </c>
       <c r="AA9" s="17"/>
       <c r="AB9" s="17"/>
-      <c r="AC9" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD9" s="34" t="s">
+      <c r="AC9" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD9" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AE9" s="34" t="s">
+      <c r="AE9" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="34"/>
-      <c r="AI9" s="34"/>
-      <c r="AJ9" s="34"/>
-      <c r="AK9" s="34"/>
-      <c r="AL9" s="34"/>
-      <c r="AM9" s="34"/>
-      <c r="AN9" s="34"/>
-      <c r="AO9" s="34" t="s">
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
+      <c r="AJ9" s="24"/>
+      <c r="AK9" s="24"/>
+      <c r="AL9" s="24"/>
+      <c r="AM9" s="24"/>
+      <c r="AN9" s="24"/>
+      <c r="AO9" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="AP9" s="34"/>
-      <c r="AQ9" s="34"/>
-      <c r="AR9" s="34"/>
-      <c r="AS9" s="34"/>
+      <c r="AP9" s="24"/>
+      <c r="AQ9" s="24"/>
+      <c r="AR9" s="24"/>
+      <c r="AS9" s="24"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="29"/>
-      <c r="C10" s="33"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
       <c r="AA10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="AB10" s="18" t="s">
+      <c r="AB10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="34"/>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="24"/>
       <c r="AE10" s="10" t="s">
         <v>58</v>
       </c>
       <c r="AF10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AG10" s="10" t="s">
+      <c r="AH10" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AH10" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="AI10" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AJ10" s="10" t="s">
+      <c r="AK10" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="AK10" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="AL10" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AM10" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AN10" s="10" t="s">
         <v>62</v>
       </c>
       <c r="AO10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP10" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AP10" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AR10" s="10" t="s">
+      <c r="AS10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AS10" s="10" t="s">
-        <v>70</v>
-      </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
@@ -1309,14 +1295,14 @@
       <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>5</v>
@@ -1334,9 +1320,9 @@
         <v>18</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="M11" s="22" t="e">
+        <v>88</v>
+      </c>
+      <c r="M11" s="14" t="e">
         <f>IF(Y11&lt;=EOMONTH(J11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
@@ -1349,19 +1335,19 @@
       <c r="P11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="22" t="e">
+      <c r="Q11" s="14" t="e">
         <f>IF(Y11&lt;=EOMONTH(J11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="22" t="e">
+      <c r="R11" s="14" t="e">
         <f>IF(AND(Y11&gt;=EOMONTH(J11,13),Y11&lt;=EOMONTH(J11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S11" s="22" t="e">
+      <c r="S11" s="14" t="e">
         <f>IF(AND(Y11&gt;=EOMONTH(J11,48),Y11&lt;=EOMONTH(J11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="T11" s="22" t="e">
+      <c r="T11" s="14" t="e">
         <f>IF(Y11&gt;=EOMONTH(J11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
@@ -1383,49 +1369,49 @@
       <c r="Z11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AA11" s="20" t="e">
+      <c r="AA11" s="19" t="e">
         <f>(EOMONTH(Y11,0))-(Y11-DAY(Y11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AB11" s="20" t="e">
+      <c r="AB11" s="19" t="e">
         <f>Z11-Y11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC11" s="20" t="s">
+      <c r="AC11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AD11" s="24" t="e">
+      <c r="AD11" s="20" t="e">
         <f>AB11/AA11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AE11" s="21" t="s">
+      <c r="AE11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="AF11" s="21" t="s">
+      <c r="AF11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG11" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="AG11" s="21" t="s">
+      <c r="AH11" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="AH11" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI11" s="21" t="s">
+      <c r="AI11" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ11" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AJ11" s="21" t="s">
+      <c r="AK11" s="20" t="s">
         <v>84</v>
-      </c>
-      <c r="AK11" s="21" t="s">
-        <v>85</v>
       </c>
       <c r="AL11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AM11" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN11" s="24" t="e">
+      <c r="AM11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN11" s="20" t="e">
         <f>AK11*AD11</f>
         <v>#VALUE!</v>
       </c>
@@ -1435,30 +1421,30 @@
       <c r="AP11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="AQ11" s="27" t="s">
+      <c r="AQ11" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="AR11" s="27" t="s">
+      <c r="AS11" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="AS11" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT11" s="26" t="s">
+      <c r="AT11" s="23" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="AE9:AN9"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:T8"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="L9:L10"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="W9:W10"/>
     <mergeCell ref="Y8:AS8"/>
@@ -1475,15 +1461,15 @@
     <mergeCell ref="AO9:AS9"/>
     <mergeCell ref="X9:X10"/>
     <mergeCell ref="U8:V8"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:T8"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="AE9:AN9"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="U9:U10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
kibon-3327: improve statistik vorlage - avoid reference error in excel formula
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kinder.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kinder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java\kibon\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5AC300-7406-40A9-B3DA-6E99233B3148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633C25EF-3091-4075-89F0-956C71816BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -534,7 +534,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -542,20 +542,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -644,9 +644,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,9 +684,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,26 +719,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -771,26 +754,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -969,7 +935,9 @@
   </sheetPr>
   <dimension ref="A1:AV11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1066,25 +1034,25 @@
       <c r="F6" s="9"/>
     </row>
     <row r="8" spans="1:48" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="33" t="s">
         <v>35</v>
       </c>
       <c r="H8" s="28" t="s">
@@ -1101,7 +1069,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
       <c r="S8" s="29"/>
-      <c r="T8" s="31"/>
+      <c r="T8" s="30"/>
       <c r="U8" s="28" t="s">
         <v>53</v>
       </c>
@@ -1110,105 +1078,105 @@
         <v>54</v>
       </c>
       <c r="X8" s="29"/>
-      <c r="Y8" s="30" t="s">
+      <c r="Y8" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
-      <c r="AB8" s="30"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="30"/>
-      <c r="AG8" s="30"/>
-      <c r="AH8" s="30"/>
-      <c r="AI8" s="30"/>
-      <c r="AJ8" s="30"/>
-      <c r="AK8" s="30"/>
-      <c r="AL8" s="30"/>
-      <c r="AM8" s="30"/>
-      <c r="AN8" s="30"/>
-      <c r="AO8" s="30"/>
-      <c r="AP8" s="30"/>
-      <c r="AQ8" s="30"/>
-      <c r="AR8" s="30"/>
-      <c r="AS8" s="30"/>
-      <c r="AT8" s="30"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
+      <c r="AF8" s="27"/>
+      <c r="AG8" s="27"/>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="27"/>
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="27"/>
+      <c r="AT8" s="27"/>
       <c r="AU8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="30" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="30" t="s">
+      <c r="I9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="30" t="s">
+      <c r="N9" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="O9" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="P9" s="33" t="s">
+      <c r="P9" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="Q9" s="30" t="s">
+      <c r="Q9" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="R9" s="30" t="s">
+      <c r="R9" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="S9" s="30" t="s">
+      <c r="S9" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="30" t="s">
+      <c r="T9" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="30" t="s">
+      <c r="U9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="V9" s="30" t="s">
+      <c r="V9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="W9" s="30" t="s">
+      <c r="W9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="X9" s="30" t="s">
+      <c r="X9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="Y9" s="30" t="s">
+      <c r="Y9" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="Z9" s="30" t="s">
+      <c r="Z9" s="27" t="s">
         <v>56</v>
       </c>
       <c r="AA9" s="17"/>
       <c r="AB9" s="17"/>
-      <c r="AC9" s="33" t="s">
+      <c r="AC9" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="AD9" s="30" t="s">
+      <c r="AD9" s="27" t="s">
         <v>57</v>
       </c>
       <c r="AE9" s="28" t="s">
@@ -1223,53 +1191,53 @@
       <c r="AL9" s="29"/>
       <c r="AM9" s="29"/>
       <c r="AN9" s="29"/>
-      <c r="AO9" s="31"/>
-      <c r="AP9" s="30" t="s">
+      <c r="AO9" s="30"/>
+      <c r="AP9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="AQ9" s="30"/>
-      <c r="AR9" s="30"/>
-      <c r="AS9" s="30"/>
-      <c r="AT9" s="30"/>
+      <c r="AQ9" s="27"/>
+      <c r="AR9" s="27"/>
+      <c r="AS9" s="27"/>
+      <c r="AT9" s="27"/>
       <c r="AU9" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
       <c r="AA10" s="17" t="s">
         <v>0</v>
       </c>
       <c r="AB10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="AC10" s="34"/>
-      <c r="AD10" s="30"/>
+      <c r="AC10" s="32"/>
+      <c r="AD10" s="27"/>
       <c r="AE10" s="10" t="s">
         <v>58</v>
       </c>
@@ -1357,9 +1325,9 @@
       <c r="L11" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="M11" s="14" t="e">
-        <f>IF(Y11&lt;=EOMONTH(J11,12),"X","")</f>
-        <v>#VALUE!</v>
+      <c r="M11" s="14" t="str">
+        <f>IF(ISNUMBER(J11),IF(Y11&lt;=EOMONTH(J11,12),"X",""),"")</f>
+        <v/>
       </c>
       <c r="N11" s="14" t="s">
         <v>19</v>
@@ -1370,21 +1338,21 @@
       <c r="P11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="14" t="e">
-        <f>IF(Y11&lt;=EOMONTH(J11,12),"X","")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R11" s="14" t="e">
-        <f>IF(AND(Y11&gt;=EOMONTH(J11,13),Y11&lt;=EOMONTH(J11,48)),"X","")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S11" s="14" t="e">
-        <f>IF(AND(Y11&gt;=EOMONTH(J11,48),Y11&lt;=EOMONTH(J11,72)),"X","")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T11" s="14" t="e">
-        <f>IF(Y11&gt;=EOMONTH(J11,73),"X","")</f>
-        <v>#VALUE!</v>
+      <c r="Q11" s="14" t="str">
+        <f>IF(ISNUMBER(J11),IF(Y11&lt;=EOMONTH(J11,12),"X",""),"")</f>
+        <v/>
+      </c>
+      <c r="R11" s="14" t="str">
+        <f>IF(ISNUMBER(J11),IF(AND(Y11&gt;=EOMONTH(J11,13),Y11&lt;=EOMONTH(J11,48)),"X",""),"")</f>
+        <v/>
+      </c>
+      <c r="S11" s="14" t="str">
+        <f>IF(ISNUMBER(J11),IF(AND(Y11&gt;=EOMONTH(J11,48),Y11&lt;=EOMONTH(J11,72)),"X",""),"")</f>
+        <v/>
+      </c>
+      <c r="T11" s="14" t="str">
+        <f>IF(ISNUMBER(J11),IF(Y11&gt;=EOMONTH(J11,73),"X",""),"")</f>
+        <v/>
       </c>
       <c r="U11" s="13" t="s">
         <v>11</v>
@@ -1446,9 +1414,9 @@
       <c r="AM11" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="AN11" s="20" t="e">
-        <f>AK11*AD11</f>
-        <v>#VALUE!</v>
+      <c r="AN11" s="20" t="str">
+        <f>IF(ISNUMBER(AK11),AK11*AD11,"")</f>
+        <v/>
       </c>
       <c r="AO11" s="20" t="s">
         <v>91</v>
@@ -1477,25 +1445,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="AP9:AT9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AE9:AO9"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="W9:W10"/>
@@ -1511,6 +1460,25 @@
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="H8:T8"/>
+    <mergeCell ref="AP9:AT9"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="AE9:AO9"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>